<commit_message>
Add sala_de_medicacao_e_internacao.json with detailed nursing care and medication protocols
</commit_message>
<xml_diff>
--- a/script-excel-para-json/input/prescricoes.xlsx
+++ b/script-excel-para-json/input/prescricoes.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1AC289667D0E8CCD/Documentos/Saúde/Prescrições/Prescrição_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2037" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD58D4C6-099C-4958-BCEC-68E9B32D6334}"/>
+  <xr:revisionPtr revIDLastSave="2396" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EFAAB7E-B676-4E43-8038-6689DBE959E8}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="5" activeTab="9" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="2" activeTab="7" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
   </bookViews>
   <sheets>
-    <sheet name="Medicamentos" sheetId="1" r:id="rId1"/>
+    <sheet name="Para_casa" sheetId="1" r:id="rId1"/>
     <sheet name="ExameFisicos" sheetId="2" r:id="rId2"/>
     <sheet name="Evolucoes" sheetId="6" r:id="rId3"/>
     <sheet name="Kit_medicamentos" sheetId="7" r:id="rId4"/>
     <sheet name="Procedimentos" sheetId="3" r:id="rId5"/>
     <sheet name="Orientacoes" sheetId="4" r:id="rId6"/>
     <sheet name="Outros" sheetId="5" r:id="rId7"/>
-    <sheet name="PortaEInternacao" sheetId="10" r:id="rId8"/>
+    <sheet name="Sala_de_medicacao_e_Internacao" sheetId="10" r:id="rId8"/>
     <sheet name="ViasDeAdministracao" sheetId="8" r:id="rId9"/>
     <sheet name="Aprazamentos" sheetId="9" r:id="rId10"/>
   </sheets>
@@ -28,6 +28,7 @@
     <definedName name="Renovação_receita" localSheetId="6">Outros!$D$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,63 +48,6 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="3">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="5"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="6"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-  <valueMetadata count="3">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-    <bk>
-      <rc t="2" v="1"/>
-    </bk>
-    <bk>
-      <rc t="2" v="2"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/python.xml><?xml version="1.0" encoding="utf-8"?>
 <python xmlns="http://schemas.microsoft.com/office/spreadsheetml/2023/python">
   <environmentDefinition id="{882DD1B0-6546-4DFA-8A08-902A380B44EA}">
@@ -121,73 +65,11 @@
 </code>
     </initialization>
   </environmentDefinition>
-  <pythonScripts>
-    <pythonScript>
-      <code>[
-  {
-    "nome": "Ceftriaxona 1g 12/12h",
-    "texto": "Ceftriaxona 1g, 1g (1 frasco), EV, 12/12h",
-    "componentes": [
-      {
-        "item": "Cloreto de sódio à 0,9%%",
-        "dose": "100",
-        "unidade": "ml"
-      }
-    ]
-  },
-  {
-    "nome": "Ceftriaxona 2g 24/24h",
-    "texto": "Ceftriaxona 1g, 2g (2 frascos), EV, 24/24h"
-  }
-]</code>
-    </pythonScript>
-    <pythonScript>
-      <code>[
-  {
-    "nome": "Fentanil 10 mcg BIC",
-    "texto": "Fentanil 50 mcg/ml, 20 ml, BIC, vazão ACM. Concentração: 10 mcg/ml",
-    "componentes":[
-      {
-        "item": "Glicose à 5%%",
-        "dose": "80",
-        "unidade": "ml"
-      }
-                  ]
-  },
-]</code>
-    </pythonScript>
-    <pythonScript>
-      <code>[
-    {
-    "nome": "Midazolam 1 mg/ml BIC (150 ml)",
-    "texto": "Midazolam 5 mg/ml, 30 ml, BIC, vazão ACM. Concentração: 1 mg/ml",
-    "componentes":[
-      {
-        "item": "SF 0,9%% ou SG 5%%",
-        "dose": "120",
-        "unidade": "ml"
-      }
-                  ]
-    },
-    {
-    "nome": "Midazolam 1 mg/ml BIC (250ml)",
-    "texto": "Midazolam 5 mg/ml, 50 ml, BIC, vazão ACM. Concentração: 1 mg/ml",
-    "componentes":[
-        {
-        "item": "SF 0,9%% ou SG 5%%",
-        "dose": "200",
-        "unidade": "ml"
-        }
-                    ]
-    },
-]</code>
-    </pythonScript>
-  </pythonScripts>
 </python>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="722">
   <si>
     <t>NomeBusca</t>
   </si>
@@ -2375,28 +2257,16 @@
     <t>Simples</t>
   </si>
   <si>
-    <t>1g/frasco</t>
-  </si>
-  <si>
     <t>g; mg</t>
   </si>
   <si>
     <t>Dieta via oral</t>
   </si>
   <si>
-    <t>Monitorização</t>
-  </si>
-  <si>
     <t>Cuidados da enfermagem</t>
   </si>
   <si>
     <t>Sinais vitais</t>
-  </si>
-  <si>
-    <t>Sinais vitais de 2 em 2 horas</t>
-  </si>
-  <si>
-    <t>Sinais vitais de 6 em 6 horas</t>
   </si>
   <si>
     <t>25 mg Comp;
@@ -2426,21 +2296,9 @@
 50 mcg/ml Amp 2 ml</t>
   </si>
   <si>
-    <t>mg; ml</t>
-  </si>
-  <si>
     <t>Cloreto de sódio</t>
   </si>
   <si>
-    <t>ml; frasco</t>
-  </si>
-  <si>
-    <t>0,9% (100 ml);
-0,9% (250 ml);
-0,9% (500 ml);
-0,9% (1000 ml);</t>
-  </si>
-  <si>
     <t>Cuidados com posicionamento</t>
   </si>
   <si>
@@ -2594,7 +2452,472 @@
     <t>Descricao</t>
   </si>
   <si>
-    <t>Correr em 30 minutos</t>
+    <t>Infundir em 30 minutos</t>
+  </si>
+  <si>
+    <t>500 mg/ml solução oral;
+500 mg/ml Amp 2 ml</t>
+  </si>
+  <si>
+    <t>ACM</t>
+  </si>
+  <si>
+    <t>À critério médico</t>
+  </si>
+  <si>
+    <t>Em jejum</t>
+  </si>
+  <si>
+    <t>Após almoço</t>
+  </si>
+  <si>
+    <t>Manhã</t>
+  </si>
+  <si>
+    <t>Tarde</t>
+  </si>
+  <si>
+    <t>Noite</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Fentanil 10 mcg BIC",
+		"texto": "Fentanil 50 mcg/ml, 20 ml, BIC, vazão ACM. Concentração: 10 mcg/ml",
+		"componentes":	[
+			{
+				"item": "Glicose à 5%",
+				"dose": "80",
+				"unidade": "ml"
+			}
+					]
+	}
+]</t>
+  </si>
+  <si>
+    <t>25 mg/ml Amp 3</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Diclofenaco 75mg agora",
+		"texto": "Diclofenaco 25 mg/ml, 3 ml, IM, agora"
+	}
+]</t>
+  </si>
+  <si>
+    <t>5 mg/ml Amp 2 ml</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Ceftriaxona 1g 12/12h",
+        "texto": "Ceftriaxona 1g, 1g (1 frasco), EV, 12/12h",
+        "componentes": [
+            {
+                "item": "Cloreto de sódio à 0,9%",
+                "dose": "100",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "Infundir em 30 minutos"
+    },
+    {
+        "nome": "Ceftriaxona 2g 24/24h",
+        "texto": "Ceftriaxona 1g, 2g (2 frascos), EV, 24/24h",
+        "componentes": [
+            {
+                "item": "Cloreto de sódio à 0,9%",
+                "dose": "100",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "Infundir em 30 minutos"
+    }
+]</t>
+  </si>
+  <si>
+    <t>25 mg/ml Amp 2 ml</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Midazolam 1 mg/ml BIC (150 ml)",
+        "texto": "Midazolam 5 mg/ml, 30 ml, BIC, vazão ACM. Concentração: 1 mg/ml",
+        "componentes": [
+            {
+                "item": "SF 0,9% ou SG 5%",
+                "dose": "120",
+                "unidade": "ml"
+            }
+        ]
+    },
+    {
+        "nome": "Midazolam 1 mg/ml BIC (250ml)",
+        "texto": "Midazolam 5 mg/ml, 50 ml, BIC, vazão ACM. Concentração: 1 mg/ml",
+        "componentes": [
+            {
+                "item": "SF 0,9% ou SG 5%",
+                "dose": "200",
+                "unidade": "ml"
+            }
+        ]
+    },
+    {
+        "nome": "Midazolam 10 mg IM agora",
+        "texto": "Midazolam 5 mg/ml, 2ml, IM, agora"
+    }
+]</t>
+  </si>
+  <si>
+    <t>20 mg/ml Amp 1 ml</t>
+  </si>
+  <si>
+    <t>1g Amp Pó</t>
+  </si>
+  <si>
+    <t>20 mg Amp pó</t>
+  </si>
+  <si>
+    <t>mg; ampola</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Tenoxicam 20mg agora",
+		"texto": "Tenoxicam 20 mg, 20 mg (1 ampola), EV, agora"
+	}
+]</t>
+  </si>
+  <si>
+    <t>4 mg/ml Amp 2,5 ml</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Dexametasona 10mg IM agora",
+		"texto": "Dexametasona 4 mg/ml, 2,5ml (1 ampola), IM, agora"
+	}
+]</t>
+  </si>
+  <si>
+    <t>Clonazepam</t>
+  </si>
+  <si>
+    <t>2,5 mg/ml Solução oral</t>
+  </si>
+  <si>
+    <t>gotas; mg</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Clonazepam  6 gotas agora",
+		"texto": "Clonazepam 2,5 mg/ml, 6 gotas, VO, agora"
+	}
+]</t>
+  </si>
+  <si>
+    <t>Diazepam</t>
+  </si>
+  <si>
+    <t>5  mg/ml Amp 2 ml</t>
+  </si>
+  <si>
+    <t>ml; mg</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Midazolam 10 mg EV agora",
+		"texto": "Midazolam 5 mg/ml, 2 ml em 10 ml de ABD, EV, lento, agora",
+		"observacao": "Infundir em 3 minutos"
+	}
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penicilina benzatina </t>
+  </si>
+  <si>
+    <t>1,2M de U Amp pó</t>
+  </si>
+  <si>
+    <t>UI; ampola</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Penicilina benzatina 1,2M UI IM agora",
+		"texto": "Penicilina benzatina 1,2 M UI, aplicar 1,2 M UI (1 ampola), IM, agora"
+	}
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insulina humana regular </t>
+  </si>
+  <si>
+    <t>100 UI/ml Amp 10 ml</t>
+  </si>
+  <si>
+    <t>UI; ml</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Insulina humana regular SC 4/4h se necessário",
+		"texto": "Insulina humana regular, SC, 4/4h, se glicemia capilar: 200-250: aplicar 2 UI / 250-300: aplicar 4 UI / 300-350: aplicar 6 UI / 350-400: aplicar 8 UI / &gt; 400: solicitar avaliação médica"
+	}
+]</t>
+  </si>
+  <si>
+    <t>Glicose</t>
+  </si>
+  <si>
+    <t>ml; ampola; L</t>
+  </si>
+  <si>
+    <t>ml; frasco; L</t>
+  </si>
+  <si>
+    <t>0,9% Bolsa 100 ml;
+0,9% Bolsa 250 ml;
+0,9% Bolsa 500 ml;
+0,9% Bolsa 1000 ml;
+20 % Amp 10 ml</t>
+  </si>
+  <si>
+    <t>50% Amp 10 ml;
+5% Bolsa 250 ml;
+5% Bolsa 500 ml;
+10% Bolsa 250 ml;
+10% Bolsa 500 ml</t>
+  </si>
+  <si>
+    <t>Restrição no leito</t>
+  </si>
+  <si>
+    <t>Repouso absoluto no leito</t>
+  </si>
+  <si>
+    <t>Repouso relativo no leito</t>
+  </si>
+  <si>
+    <t>Contenção física no leito</t>
+  </si>
+  <si>
+    <t>Controle glicêmico</t>
+  </si>
+  <si>
+    <t>Controles glicêmicos a cada 4/4h</t>
+  </si>
+  <si>
+    <t>Acído acetilsalicílico</t>
+  </si>
+  <si>
+    <t>100 mg Comp</t>
+  </si>
+  <si>
+    <t>mg; comp</t>
+  </si>
+  <si>
+    <t>Clopidogrel</t>
+  </si>
+  <si>
+    <t>75 mg Comp</t>
+  </si>
+  <si>
+    <t>Amiodarona</t>
+  </si>
+  <si>
+    <t>50 mg/ml Amp 3 ml</t>
+  </si>
+  <si>
+    <t>Atropina</t>
+  </si>
+  <si>
+    <t>0,25 mg/ml Amp 1 ml;
+0,5 mg/ml Amp 1ml</t>
+  </si>
+  <si>
+    <t>Adenosina</t>
+  </si>
+  <si>
+    <t>3 mg/ml Ampo 2 ml</t>
+  </si>
+  <si>
+    <t>100 mcg</t>
+  </si>
+  <si>
+    <t>mcg; jatos</t>
+  </si>
+  <si>
+    <t>0,25 mg/ml Solução para nebulização</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidrocortisona </t>
+  </si>
+  <si>
+    <t>100 mg Amp pó</t>
+  </si>
+  <si>
+    <t>mg, ampola</t>
+  </si>
+  <si>
+    <t>Sulfato de magnésio</t>
+  </si>
+  <si>
+    <t>10% Amp 10 ml;
+20% Amp 10 ml;
+50% Amp 10 ml</t>
+  </si>
+  <si>
+    <t>Morfina</t>
+  </si>
+  <si>
+    <t>10 mg/ml Amp 1 ml</t>
+  </si>
+  <si>
+    <t>Carvão ativado</t>
+  </si>
+  <si>
+    <t>25 g Envelope</t>
+  </si>
+  <si>
+    <t>g; envelope</t>
+  </si>
+  <si>
+    <t>Cloreto de potássio</t>
+  </si>
+  <si>
+    <t>10% Amp 10 ml;
+19,1% Amp 10 ml</t>
+  </si>
+  <si>
+    <t>ml; mg; ampola</t>
+  </si>
+  <si>
+    <t>ml; mg; g; ampola</t>
+  </si>
+  <si>
+    <t>gotas; ml; mg</t>
+  </si>
+  <si>
+    <t>mg; ml; ampola</t>
+  </si>
+  <si>
+    <t>Haloperidol</t>
+  </si>
+  <si>
+    <t>5 mg/ml Amp 1 ml</t>
+  </si>
+  <si>
+    <t>Norepinefrina</t>
+  </si>
+  <si>
+    <t>1 mg/ml Amp 4 ml</t>
+  </si>
+  <si>
+    <t>Nitroprussiato</t>
+  </si>
+  <si>
+    <t>Dobutamina</t>
+  </si>
+  <si>
+    <t>12,5 mg/ml Amp 20 ml</t>
+  </si>
+  <si>
+    <t>Dopamina</t>
+  </si>
+  <si>
+    <t>5 mg/ml Amp 10 ml</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Bromoprida 10 mg agora",
+		"texto": "Bromoprida 5 mg/ml, 2ml, EV, agora"
+	},
+	{
+		"nome": "Bromoprida 10 mg 6/6h se necessário",
+		"texto": "Bromoprida 5 mg/ml, 2 ml, EV, 8/8h, se náuseas ou vômitos"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Dipirona 1g agora",
+		"texto": "Dipirona 500 mg/ml, 2ml, EV, agora"
+	},
+	{
+		"nome": "Dipirona 1g 6/6h se necessário",
+		"texto": "Dipirona 500 mg/ml, 2 ml, EV, de 6/6h, se dor ou febre"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Escopolamina 20 mg agora",
+		"texto": "Escopolamina 20 mg/ml, 1 ml, EV, agora"
+	},
+	{
+		"nome": "Escopolamina 20 mg 6/6h se necessário",
+		"texto": "Escopolamina 20 mg/ml, 1 ml, EV, 6/6h, se dor abdominal"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Prometazina 50 mg IM agora",
+		"texto": "Prometazina 25 mg/ml, 2ml, IM, agora"
+	},
+	{
+		"nome": "Prometazina 50 mg IM 12/12h",
+		"texto": "Prometazina 25 mg/ml, 2ml, IM, 12/12h"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Glicose à 50% 40 ml EV agora",
+		"texto": "Glicose à 50%, 40 ml, EV, bolus, se HGT &lt; 70. Observação: comunicar o médico"
+	},
+	{
+		"nome": "Glicose à 50% 40 ml EV se necessário",
+		"texto": "Glicose à 50%, 40 ml, EV, bolus, se HGT &lt; 70" ,
+		"observacao": "comunicar o médico(a)"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Metoclopramida 10 mg agora",
+		"texto": "Metoclopramida 5 mg/ml, 2ml em 8 ml de ABD, EV, lento, agora"
+	},
+	{
+		"nome": "Metoclopramida 10 mg 8/8h se necessário",
+		"texto": "Metoclopramida 5 mg/ml, 2 ml diluído em 8 ml de ABD, EV, lento, 8/8h, se náuseas ou vômitos"
+	}
+]</t>
+  </si>
+  <si>
+    <t>Aferir sinais vitais</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "SSVV 2/2h",
+		"texto": "Aferir sinais vitais de 2 em 2 horas"
+	},
+	{
+		"nome": "SSVV 6/6h",
+		"texto": "Aferir sinais vitais de 6 em 6 horas"
+	}
+]</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2963,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2659,8 +2982,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2716,11 +3045,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2771,20 +3109,302 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2855,18 +3475,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3146,6 +3754,18 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3163,183 +3783,20 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
-<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="2">
-  <a r="2">
-    <v t="s">&lt;dict&gt;</v>
-    <v t="s">&lt;dict&gt;</v>
-  </a>
-  <a r="1">
-    <v t="s">&lt;dict&gt;</v>
-  </a>
-</arrayData>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
-  <rv s="0">
-    <v>0</v>
-  </rv>
-  <rv s="1">
-    <v>list</v>
-    <v>1</v>
-    <v>0</v>
-  </rv>
-  <rv s="2">
-    <v>&lt;class 'list'&gt;</v>
-    <v>list</v>
-    <v>[{'nome': 'Ceftriaxona 1g 12/12h', 'texto': 'Ceftriaxona 1g, 1g (1 frasco), EV, 12/12h', 'componentes': [{'item': 'Cloreto de sódio à 0,9%', 'dose': '100', 'unidade': 'ml'}]}, {'nome': 'Ceftriaxona 2g 24/24h', 'texto': 'Ceftriaxona 1g, 2g (2 frascos), ...</v>
-    <v>1</v>
-    <v>2</v>
-  </rv>
-  <rv s="0">
-    <v>1</v>
-  </rv>
-  <rv s="1">
-    <v>list</v>
-    <v>4</v>
-    <v>3</v>
-  </rv>
-  <rv s="2">
-    <v>&lt;class 'list'&gt;</v>
-    <v>list</v>
-    <v>[{'nome': 'Fentanil 10 mcg BIC', 'texto': 'Fentanil 50 mcg/ml, 20 ml, BIC, vazão ACM. Concentração: 10 mcg/ml', 'componentes': [{'item': 'Glicose à 5%', 'dose': '80', 'unidade': 'ml'}]}]</v>
-    <v>4</v>
-    <v>2</v>
-  </rv>
-  <rv s="2">
-    <v>&lt;class 'list'&gt;</v>
-    <v>list</v>
-    <v>[{'nome': 'Midazolam 1 mg/ml BIC (150 ml)', 'texto': 'Midazolam 5 mg/ml, 30 ml, BIC, vazão ACM. Concentração: 1 mg/ml', 'componentes': [{'item': 'SF 0,9% ou SG 5%', 'dose': '120', 'unidade': 'ml'}]}, {'nome': 'Midazolam 1 mg/ml BIC (250ml)', 'texto': '...</v>
-    <v>1</v>
-    <v>2</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
-  <s t="_array">
-    <k n="array" t="a"/>
-  </s>
-  <s t="_entity">
-    <k n="_DisplayString" t="s"/>
-    <k n="_ViewInfo" t="spb"/>
-    <k n="arrayPreview" t="r"/>
-  </s>
-  <s t="_python">
-    <k n="Python_type" t="s"/>
-    <k n="Python_typeName" t="s"/>
-    <k n="Python_str" t="s"/>
-    <k n="preview" t="r"/>
-    <k n="_Provider" t="spb"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
-<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbData count="5">
-    <spb s="0">
-      <v>2</v>
-      <v>1</v>
-      <v>list</v>
-      <v>arrayPreview</v>
-    </spb>
-    <spb s="1">
-      <v>0</v>
-    </spb>
-    <spb s="2">
-      <v>https://www.anaconda.com/excel</v>
-      <v>https://res.cdn.office.net/officepysvc/prod-preview/anacondalogo.png</v>
-      <v>Python fornecido por Anaconda</v>
-    </spb>
-    <spb s="0">
-      <v>1</v>
-      <v>1</v>
-      <v>list</v>
-      <v>arrayPreview</v>
-    </spb>
-    <spb s="1">
-      <v>3</v>
-    </spb>
-  </spbData>
-</supportingPropertyBags>
-</file>
-
-<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="3">
-  <s>
-    <k n="drw" t="i"/>
-    <k n="dcol" t="i"/>
-    <k n="name" t="s"/>
-    <k n="array" t="s"/>
-  </s>
-  <s>
-    <k n="ArrayCardInfo" t="spb"/>
-  </s>
-  <s>
-    <k n="link" t="s"/>
-    <k n="logo" t="s"/>
-    <k n="name" t="s"/>
-  </s>
-</spbStructures>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}" name="Tabela1" displayName="Tabela1" ref="A1:V159" totalsRowShown="0">
   <autoFilter ref="A1:V159" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V158">
-    <sortCondition ref="B1:B158"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V159">
+    <sortCondition ref="B1:B159"/>
   </sortState>
   <tableColumns count="22">
     <tableColumn id="7" xr3:uid="{EEA224EE-B017-42F5-A417-487E2B86AD5D}" name="ID_Item">
       <calculatedColumnFormula>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{FF9AC4B3-0AB1-43C0-813C-9F0FBFCD27C3}" name="NomeBusca" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A4280A1D-29DF-4DF8-BAEB-74D735392255}" name="PrescricaoCompleta" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{1C09888C-F0B3-445C-96A7-59EF6CBB8977}" name="Categoria" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{E1DAEFD1-96A5-4769-95CA-789E157CF235}" name="Doenca" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{FF9AC4B3-0AB1-43C0-813C-9F0FBFCD27C3}" name="NomeBusca" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{A4280A1D-29DF-4DF8-BAEB-74D735392255}" name="PrescricaoCompleta" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{1C09888C-F0B3-445C-96A7-59EF6CBB8977}" name="Categoria" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{E1DAEFD1-96A5-4769-95CA-789E157CF235}" name="Doenca" dataDxfId="54"/>
     <tableColumn id="5" xr3:uid="{00D107C9-5770-4523-8A77-BC2E8CCDFA3F}" name="OrdemPrioridade"/>
     <tableColumn id="6" xr3:uid="{A2A03C33-701E-4A02-84BD-0D3C40E0270C}" name="FormaFarmaceutica"/>
     <tableColumn id="8" xr3:uid="{037F36DC-527F-4AE8-A6F4-3169AA433215}" name="isCalculable"/>
@@ -3363,8 +3820,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9BC025B4-0C86-43DA-9BA8-AD95BA9033CF}" name="Tabela7" displayName="Tabela7" ref="A1:B20" totalsRowShown="0">
-  <autoFilter ref="A1:B20" xr:uid="{9BC025B4-0C86-43DA-9BA8-AD95BA9033CF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9BC025B4-0C86-43DA-9BA8-AD95BA9033CF}" name="Tabela7" displayName="Tabela7" ref="A1:B26" totalsRowShown="0">
+  <autoFilter ref="A1:B26" xr:uid="{9BC025B4-0C86-43DA-9BA8-AD95BA9033CF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CFD77929-9554-43BE-908D-A85767D19E05}" name="Horario"/>
     <tableColumn id="2" xr3:uid="{371D9874-4C27-4E8A-9C60-1E16D092C8FD}" name="Descricao"/>
@@ -3374,131 +3831,134 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B1BCF4E-F9B8-4BCA-9A1B-734209B09515}" name="Tabela2" displayName="Tabela2" ref="A1:E6" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B1BCF4E-F9B8-4BCA-9A1B-734209B09515}" name="Tabela2" displayName="Tabela2" ref="A1:E6" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:E6" xr:uid="{7B1BCF4E-F9B8-4BCA-9A1B-734209B09515}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{3B85112C-C948-4532-A5A9-B2DC134B2714}" name="ID_Item" dataDxfId="44">
+    <tableColumn id="5" xr3:uid="{3B85112C-C948-4532-A5A9-B2DC134B2714}" name="ID_Item" dataDxfId="51">
       <calculatedColumnFormula>ROW() - ROW(Tabela2[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{294ACE13-D92E-4E83-AE9A-884FBB3BAD21}" name="NomeBusca" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{57C4FF43-CE4E-4A4E-A745-1D12588CAE36}" name="ConteudoTexto" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{1B0E7410-6713-475C-9274-E8D53C220050}" name="Categoria" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{E775B5FA-D905-41A5-AF49-15CA3264FA30}" name="OrdemPrioridade" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{294ACE13-D92E-4E83-AE9A-884FBB3BAD21}" name="NomeBusca" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{57C4FF43-CE4E-4A4E-A745-1D12588CAE36}" name="ConteudoTexto" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{1B0E7410-6713-475C-9274-E8D53C220050}" name="Categoria" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{E775B5FA-D905-41A5-AF49-15CA3264FA30}" name="OrdemPrioridade" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F1B6F081-4196-40D7-9E1B-E18AC00A544A}" name="Tabela57" displayName="Tabela57" ref="A1:E9" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F1B6F081-4196-40D7-9E1B-E18AC00A544A}" name="Tabela57" displayName="Tabela57" ref="A1:E9" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:E9" xr:uid="{F1B6F081-4196-40D7-9E1B-E18AC00A544A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
     <sortCondition ref="E1:E9"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{255D6023-30BF-414A-B3B5-09A8AED4AD40}" name="ID_Item" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{255D6023-30BF-414A-B3B5-09A8AED4AD40}" name="ID_Item" dataDxfId="44">
       <calculatedColumnFormula>ROW() - ROW(Tabela57[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{8C75D187-576A-41EF-9BC9-337001D161C6}" name="NomeBusca" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{7A836061-FA92-4D6E-A1CB-B0A3080FF4E2}" name="ConteudoTexto" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{9C7516CD-131C-4A90-BC19-727B1919928E}" name="Categoria" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{D9BE6F3B-192E-46DB-ADBD-41AC809A383A}" name="OrdemPrioridade" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{8C75D187-576A-41EF-9BC9-337001D161C6}" name="NomeBusca" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{7A836061-FA92-4D6E-A1CB-B0A3080FF4E2}" name="ConteudoTexto" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{9C7516CD-131C-4A90-BC19-727B1919928E}" name="Categoria" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{D9BE6F3B-192E-46DB-ADBD-41AC809A383A}" name="OrdemPrioridade" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}" name="Tabela8" displayName="Tabela8" ref="A1:E6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}" name="Tabela8" displayName="Tabela8" ref="A1:E6" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:E6" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C07F2220-FEC5-4C0B-AB14-F80860FCB6A0}" name="ID_Item" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{C07F2220-FEC5-4C0B-AB14-F80860FCB6A0}" name="ID_Item" dataDxfId="37">
       <calculatedColumnFormula>ROW() - ROW(Tabela5[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F6AB2AED-7D50-4A14-A3D8-3D697CD7C3E6}" name="NomeBusca" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{24DCE466-5828-477A-94D8-8B94F125CA52}" name="ConteudoTexto" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{544BC52C-0699-476B-9E91-F8010861B484}" name="Categoria" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{0A44EF13-A692-417E-90F4-EEE1E0C399BB}" name="OrdemPrioridade" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{F6AB2AED-7D50-4A14-A3D8-3D697CD7C3E6}" name="NomeBusca" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{24DCE466-5828-477A-94D8-8B94F125CA52}" name="ConteudoTexto" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{544BC52C-0699-476B-9E91-F8010861B484}" name="Categoria" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{0A44EF13-A692-417E-90F4-EEE1E0C399BB}" name="OrdemPrioridade" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B195B058-C443-4C22-BFDA-1A6D6B3BD53F}" name="Tabela3" displayName="Tabela3" ref="A1:D7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B195B058-C443-4C22-BFDA-1A6D6B3BD53F}" name="Tabela3" displayName="Tabela3" ref="A1:D7" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:D7" xr:uid="{B195B058-C443-4C22-BFDA-1A6D6B3BD53F}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{30594E46-81AD-44D9-A464-0DDB2405FA5F}" name="ID_Item" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{30594E46-81AD-44D9-A464-0DDB2405FA5F}" name="ID_Item" dataDxfId="30">
       <calculatedColumnFormula>ROW() - ROW(Tabela3[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{CC635276-E45D-489A-B013-B9CB28D05F73}" name="NomeBusca" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{C4152665-161D-4E06-A92A-C044706FA22B}" name="ConteudoTexto" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{D73DEA13-D731-4A85-9704-AF815ADF8ECA}" name="Categoria" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{CC635276-E45D-489A-B013-B9CB28D05F73}" name="NomeBusca" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{C4152665-161D-4E06-A92A-C044706FA22B}" name="ConteudoTexto" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{D73DEA13-D731-4A85-9704-AF815ADF8ECA}" name="Categoria" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BF31387E-C94D-4214-90A7-3EA03A21E459}" name="Tabela4" displayName="Tabela4" ref="A1:D8" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BF31387E-C94D-4214-90A7-3EA03A21E459}" name="Tabela4" displayName="Tabela4" ref="A1:D8" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:D8" xr:uid="{BF31387E-C94D-4214-90A7-3EA03A21E459}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{B03251EF-71D3-4778-9397-49B077E4BE95}" name="ID_Item" dataDxfId="17">
+    <tableColumn id="4" xr3:uid="{B03251EF-71D3-4778-9397-49B077E4BE95}" name="ID_Item" dataDxfId="24">
       <calculatedColumnFormula>ROW() - ROW(Tabela4[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{4E29BBAD-C1D6-4B95-B61D-6D2ACC75817D}" name="NomeBusca" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{E987E83A-5D1B-4FBA-B949-173B3B767BC5}" name="ConteudoTexto" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{5CEF5F95-0ACE-4A9D-B37D-26E33FA9BC59}" name="Categoria" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{4E29BBAD-C1D6-4B95-B61D-6D2ACC75817D}" name="NomeBusca" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{E987E83A-5D1B-4FBA-B949-173B3B767BC5}" name="ConteudoTexto" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{5CEF5F95-0ACE-4A9D-B37D-26E33FA9BC59}" name="Categoria" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}" name="Tabela5" displayName="Tabela5" ref="A1:E8" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}" name="Tabela5" displayName="Tabela5" ref="A1:E8" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:E8" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
     <sortCondition ref="E1:E8"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{FE4827F2-FADA-4522-96C6-C15115BA8429}" name="ID_Item" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{FE4827F2-FADA-4522-96C6-C15115BA8429}" name="ID_Item" dataDxfId="18">
       <calculatedColumnFormula>ROW() - ROW(Tabela5[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{2E3E19EF-E8C4-4174-A6DD-FE62A883B65B}" name="NomeBusca" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A403427C-6D7B-4CAC-8A29-52B0496C1B55}" name="ConteudoTexto" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{495ABE71-9083-4D12-B7AF-769A1DE8A329}" name="Categoria" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{B52F07B3-9EB3-4432-9961-0DC5F0D7CABC}" name="OrdemPrioridade" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{2E3E19EF-E8C4-4174-A6DD-FE62A883B65B}" name="NomeBusca" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{A403427C-6D7B-4CAC-8A29-52B0496C1B55}" name="ConteudoTexto" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{495ABE71-9083-4D12-B7AF-769A1DE8A329}" name="Categoria" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{B52F07B3-9EB3-4432-9961-0DC5F0D7CABC}" name="OrdemPrioridade" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{ACBDBD77-4F47-4470-9066-42382BF03E43}" name="Tabela10" displayName="Tabela10" ref="A1:I13" totalsRowShown="0">
-  <autoFilter ref="A1:I13" xr:uid="{ACBDBD77-4F47-4470-9066-42382BF03E43}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4B1D6705-EEC4-44EF-9410-0F0CC297D1AF}" name="Tabela11" displayName="Tabela11" ref="A1:I45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A1:I45" xr:uid="{4B1D6705-EEC4-44EF-9410-0F0CC297D1AF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I45">
+    <sortCondition ref="B1:B45"/>
+  </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{CF3203F3-4CFD-4D66-B74A-BC12D8F80FFA}" name="ID">
-      <calculatedColumnFormula>ROW() - ROW(Tabela10[[#Headers],[ID]])</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{301BA950-EFFF-4FE5-9DB9-5861171DCD47}" name="ID" dataDxfId="7">
+      <calculatedColumnFormula>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F0A4A9FD-374C-4C54-BB2A-5F28D41CC94F}" name="Categoria"/>
-    <tableColumn id="3" xr3:uid="{FFABFB1D-C8F4-405B-AEE9-D9AD9763CC53}" name="ItemPrincipal"/>
-    <tableColumn id="4" xr3:uid="{A34F1342-A7E3-4126-AD78-872FBDC5E7F9}" name="TipoItem"/>
-    <tableColumn id="5" xr3:uid="{713B817B-AFCD-41AC-9811-678098C3DAA2}" name="Apresentacoes"/>
-    <tableColumn id="6" xr3:uid="{51FD07B6-C473-44E8-86E2-4ADD006B84FE}" name="UnidadesDose"/>
-    <tableColumn id="7" xr3:uid="{27DD1729-7493-4AFC-BA0D-C3C0C3F7994C}" name="DescricaoCompleta"/>
-    <tableColumn id="8" xr3:uid="{25028A68-0087-4AD4-8FAB-FDB2744115FA}" name="PrescricoesPadronizadasJSON"/>
-    <tableColumn id="9" xr3:uid="{78D527DD-27A2-4C60-B2BB-5C8F58225E77}" name="ObservacaoPadrao"/>
+    <tableColumn id="2" xr3:uid="{95B7D018-E9AC-491D-B435-1F6EB200D80A}" name="Categoria" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{7CAFE1FE-9E4E-49EE-A066-49EF442BD903}" name="ItemPrincipal" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{32EB61CF-E015-4D3D-B756-51398F6C009A}" name="TipoItem" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{936FB20C-D115-4667-97E7-E129A658386C}" name="Apresentacoes"/>
+    <tableColumn id="6" xr3:uid="{DABD4860-46A3-4322-9CEC-02C728F8C85E}" name="UnidadesDose" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{F99AE901-6D2A-4AAF-A051-717D622F48E0}" name="DescricaoCompleta" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{33992999-473F-4B43-8EE4-B2F7493B3B68}" name="PrescricoesPadronizadasJSON" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{8FC9313B-C050-471A-AF80-B95E43A2F6F3}" name="ObservacaoPadrao" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{08C68780-8D11-4E55-B88C-5F8138D4CC5D}" name="Tabela9" displayName="Tabela9" ref="A1:B12" totalsRowShown="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{08C68780-8D11-4E55-B88C-5F8138D4CC5D}" name="Tabela9" displayName="Tabela9" ref="A1:B12" totalsRowShown="0" tableBorderDxfId="13">
   <autoFilter ref="A1:B12" xr:uid="{08C68780-8D11-4E55-B88C-5F8138D4CC5D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{150208FE-C1A4-49E1-81FF-1AA10AF0B961}" name="Sigla" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{79FC3213-8BF9-487D-8478-621C9C80380A}" name="Nome" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{150208FE-C1A4-49E1-81FF-1AA10AF0B961}" name="Sigla" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{79FC3213-8BF9-487D-8478-621C9C80380A}" name="Nome" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3825,7 +4285,7 @@
   <dimension ref="A1:V159"/>
   <sheetViews>
     <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6684,19 +7144,19 @@
         <v>100</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>196</v>
+        <v>38</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>395</v>
+        <v>536</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>197</v>
+        <v>39</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="G101" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H101" t="s">
         <v>500</v>
@@ -6711,7 +7171,7 @@
         <v>196</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>197</v>
@@ -6726,28 +7186,25 @@
         <v>500</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A103">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>433</v>
+        <v>196</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F103">
-        <v>4</v>
+        <v>198</v>
       </c>
       <c r="G103" t="s">
-        <v>303</v>
+        <v>256</v>
       </c>
       <c r="H103" t="s">
         <v>500</v>
@@ -6758,11 +7215,11 @@
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>103</v>
       </c>
-      <c r="B104" s="9" t="s">
-        <v>158</v>
+      <c r="B104" s="4" t="s">
+        <v>433</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>322</v>
+        <v>397</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>137</v>
@@ -6771,37 +7228,37 @@
         <v>138</v>
       </c>
       <c r="F104">
+        <v>4</v>
+      </c>
+      <c r="G104" t="s">
+        <v>303</v>
+      </c>
+      <c r="H104" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>104</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F105">
         <v>3</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G105" t="s">
         <v>298</v>
-      </c>
-      <c r="H104" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>104</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-      <c r="G105" t="s">
-        <v>256</v>
       </c>
       <c r="H105" t="s">
         <v>500</v>
@@ -6816,7 +7273,7 @@
         <v>242</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>228</v>
@@ -6834,7 +7291,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A107">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>106</v>
@@ -6843,7 +7300,7 @@
         <v>242</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>228</v>
@@ -6861,22 +7318,25 @@
         <v>500</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A108">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>107</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>140</v>
+        <v>242</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>47</v>
+        <v>228</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>48</v>
+        <v>224</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
       </c>
       <c r="G108" t="s">
         <v>256</v>
@@ -6891,16 +7351,16 @@
         <v>108</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>202</v>
+        <v>47</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>198</v>
+        <v>48</v>
       </c>
       <c r="G109" t="s">
         <v>256</v>
@@ -6915,16 +7375,16 @@
         <v>109</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>56</v>
+        <v>201</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>52</v>
+        <v>202</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="G110" t="s">
         <v>256</v>
@@ -6942,16 +7402,16 @@
         <v>56</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G111" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="H111" t="s">
         <v>500</v>
@@ -6963,13 +7423,13 @@
         <v>111</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>120</v>
@@ -6987,19 +7447,19 @@
         <v>112</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>507</v>
+        <v>118</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>508</v>
+        <v>405</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>509</v>
+        <v>119</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>512</v>
+        <v>120</v>
       </c>
       <c r="G113" t="s">
-        <v>513</v>
+        <v>254</v>
       </c>
       <c r="H113" t="s">
         <v>500</v>
@@ -7014,7 +7474,7 @@
         <v>507</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>509</v>
@@ -7038,7 +7498,7 @@
         <v>507</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>509</v>
@@ -7053,7 +7513,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A116">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>115</v>
@@ -7062,7 +7522,7 @@
         <v>507</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>509</v>
@@ -7071,82 +7531,79 @@
         <v>512</v>
       </c>
       <c r="G116" t="s">
+        <v>513</v>
+      </c>
+      <c r="H116" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>116</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="G117" t="s">
         <v>296</v>
       </c>
-      <c r="H116" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>116</v>
-      </c>
-      <c r="B117" s="4" t="s">
+      <c r="H117" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>117</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D118" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G118" t="s">
         <v>254</v>
       </c>
-      <c r="H117" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>117</v>
-      </c>
-      <c r="B118" s="4" t="s">
+      <c r="H118" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>118</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D119" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G118" t="s">
+      <c r="G119" t="s">
         <v>299</v>
-      </c>
-      <c r="H118" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>118</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D119" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F119">
-        <v>3</v>
-      </c>
-      <c r="G119" t="s">
-        <v>256</v>
       </c>
       <c r="H119" t="s">
         <v>500</v>
@@ -7161,7 +7618,7 @@
         <v>11</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>10</v>
@@ -7185,19 +7642,22 @@
         <v>120</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="F121">
+        <v>3</v>
       </c>
       <c r="G121" t="s">
-        <v>293</v>
+        <v>256</v>
       </c>
       <c r="H121" t="s">
         <v>500</v>
@@ -7209,22 +7669,19 @@
         <v>121</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F122">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G122" t="s">
-        <v>256</v>
+        <v>293</v>
       </c>
       <c r="H122" t="s">
         <v>500</v>
@@ -7236,16 +7693,19 @@
         <v>122</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>240</v>
+        <v>127</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>211</v>
+        <v>10</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>212</v>
+        <v>19</v>
+      </c>
+      <c r="F123">
+        <v>3</v>
       </c>
       <c r="G123" t="s">
         <v>256</v>
@@ -7260,16 +7720,16 @@
         <v>123</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>61</v>
+        <v>240</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>60</v>
+        <v>212</v>
       </c>
       <c r="G124" t="s">
         <v>256</v>
@@ -7278,52 +7738,52 @@
         <v>500</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A125">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>124</v>
       </c>
       <c r="B125" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G125" t="s">
+        <v>256</v>
+      </c>
+      <c r="H125" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>125</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C126" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="D125" s="4" t="s">
+      <c r="D126" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F125">
+      <c r="F126">
         <v>1</v>
       </c>
-      <c r="G125" t="s">
+      <c r="G126" t="s">
         <v>286</v>
-      </c>
-      <c r="H125" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>125</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="D126" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G126" t="s">
-        <v>300</v>
       </c>
       <c r="H126" t="s">
         <v>500</v>
@@ -7335,19 +7795,19 @@
         <v>126</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>141</v>
+        <v>2</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>414</v>
+        <v>320</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="G127" t="s">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="H127" t="s">
         <v>500</v>
@@ -7362,7 +7822,7 @@
         <v>141</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>480</v>
+        <v>414</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>47</v>
@@ -7383,19 +7843,16 @@
         <v>128</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>7</v>
+        <v>141</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>415</v>
+        <v>480</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F129">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G129" t="s">
         <v>256</v>
@@ -7413,7 +7870,7 @@
         <v>7</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>9</v>
@@ -7431,7 +7888,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A131">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>130</v>
@@ -7440,55 +7897,22 @@
         <v>7</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>494</v>
+        <v>416</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>466</v>
+        <v>19</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
       </c>
       <c r="G131" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H131" t="s">
-        <v>499</v>
-      </c>
-      <c r="I131" t="s">
-        <v>467</v>
-      </c>
-      <c r="J131" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="K131">
-        <v>10</v>
-      </c>
-      <c r="L131">
-        <v>15</v>
-      </c>
-      <c r="M131">
-        <v>200</v>
-      </c>
-      <c r="N131" t="s">
-        <v>487</v>
-      </c>
-      <c r="O131">
-        <v>20</v>
-      </c>
-      <c r="P131">
-        <v>6</v>
-      </c>
-      <c r="R131">
-        <v>75</v>
-      </c>
-      <c r="S131">
-        <v>4000</v>
-      </c>
-      <c r="T131" t="s">
-        <v>469</v>
-      </c>
-      <c r="U131" t="s">
-        <v>477</v>
+        <v>500</v>
       </c>
     </row>
     <row r="132" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -7497,28 +7921,61 @@
         <v>131</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>276</v>
+        <v>7</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>417</v>
+        <v>494</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F132">
-        <v>1</v>
+        <v>466</v>
       </c>
       <c r="G132" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H132" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="133" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+      <c r="I132" t="s">
+        <v>467</v>
+      </c>
+      <c r="J132" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="K132">
+        <v>10</v>
+      </c>
+      <c r="L132">
+        <v>15</v>
+      </c>
+      <c r="M132">
+        <v>200</v>
+      </c>
+      <c r="N132" t="s">
+        <v>487</v>
+      </c>
+      <c r="O132">
+        <v>20</v>
+      </c>
+      <c r="P132">
+        <v>6</v>
+      </c>
+      <c r="R132">
+        <v>75</v>
+      </c>
+      <c r="S132">
+        <v>4000</v>
+      </c>
+      <c r="T132" t="s">
+        <v>469</v>
+      </c>
+      <c r="U132" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A133">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>132</v>
@@ -7527,7 +7984,7 @@
         <v>276</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>9</v>
@@ -7545,49 +8002,52 @@
         <v>500</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A134">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>133</v>
       </c>
       <c r="B134" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+      <c r="G134" t="s">
+        <v>256</v>
+      </c>
+      <c r="H134" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>134</v>
+      </c>
+      <c r="B135" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="C134" s="3" t="s">
+      <c r="C135" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D135" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="E134" s="1" t="s">
+      <c r="E135" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="G134" t="s">
+      <c r="G135" t="s">
         <v>257</v>
-      </c>
-      <c r="H134" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="135" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>134</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D135" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G135" t="s">
-        <v>301</v>
       </c>
       <c r="H135" t="s">
         <v>500</v>
@@ -7599,25 +8059,25 @@
         <v>135</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>206</v>
+        <v>126</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="G136" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="H136" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A137">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>136</v>
@@ -7626,7 +8086,7 @@
         <v>174</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>206</v>
@@ -7635,31 +8095,31 @@
         <v>207</v>
       </c>
       <c r="G137" t="s">
+        <v>294</v>
+      </c>
+      <c r="H137" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>137</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G138" t="s">
         <v>292</v>
-      </c>
-      <c r="H137" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="138" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>137</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D138" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G138" t="s">
-        <v>302</v>
       </c>
       <c r="H138" t="s">
         <v>500</v>
@@ -7671,19 +8131,19 @@
         <v>138</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>323</v>
+        <v>160</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="G139" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="H139" t="s">
         <v>500</v>
@@ -7698,55 +8158,19 @@
         <v>186</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>495</v>
+        <v>323</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>481</v>
+        <v>124</v>
       </c>
       <c r="G140" t="s">
-        <v>257</v>
+        <v>290</v>
       </c>
       <c r="H140" t="s">
-        <v>499</v>
-      </c>
-      <c r="I140" t="s">
-        <v>467</v>
-      </c>
-      <c r="J140" t="s">
-        <v>482</v>
-      </c>
-      <c r="K140">
-        <v>1</v>
-      </c>
-      <c r="L140">
-        <v>2</v>
-      </c>
-      <c r="M140">
-        <v>3</v>
-      </c>
-      <c r="N140" t="s">
-        <v>473</v>
-      </c>
-      <c r="P140">
-        <v>24</v>
-      </c>
-      <c r="Q140">
-        <v>60</v>
-      </c>
-      <c r="R140">
-        <v>2</v>
-      </c>
-      <c r="S140">
-        <v>60</v>
-      </c>
-      <c r="T140" t="s">
-        <v>469</v>
-      </c>
-      <c r="U140" t="s">
-        <v>477</v>
+        <v>500</v>
       </c>
     </row>
     <row r="141" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -7755,22 +8179,58 @@
         <v>140</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>448</v>
+        <v>495</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>208</v>
+        <v>481</v>
       </c>
       <c r="G141" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H141" t="s">
-        <v>500</v>
+        <v>499</v>
+      </c>
+      <c r="I141" t="s">
+        <v>467</v>
+      </c>
+      <c r="J141" t="s">
+        <v>482</v>
+      </c>
+      <c r="K141">
+        <v>1</v>
+      </c>
+      <c r="L141">
+        <v>2</v>
+      </c>
+      <c r="M141">
+        <v>3</v>
+      </c>
+      <c r="N141" t="s">
+        <v>473</v>
+      </c>
+      <c r="P141">
+        <v>24</v>
+      </c>
+      <c r="Q141">
+        <v>60</v>
+      </c>
+      <c r="R141">
+        <v>2</v>
+      </c>
+      <c r="S141">
+        <v>60</v>
+      </c>
+      <c r="T141" t="s">
+        <v>469</v>
+      </c>
+      <c r="U141" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="142" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -7782,13 +8242,13 @@
         <v>28</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>422</v>
+        <v>448</v>
       </c>
       <c r="D142" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>30</v>
+        <v>208</v>
       </c>
       <c r="G142" t="s">
         <v>256</v>
@@ -7806,16 +8266,16 @@
         <v>28</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D143" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>534</v>
+        <v>30</v>
       </c>
       <c r="G143" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H143" t="s">
         <v>500</v>
@@ -7827,49 +8287,46 @@
         <v>143</v>
       </c>
       <c r="B144" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G144" t="s">
+        <v>257</v>
+      </c>
+      <c r="H144" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>144</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C144" s="3" t="s">
+      <c r="C145" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D145" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E144" s="1" t="s">
+      <c r="E145" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F144">
+      <c r="F145">
         <v>2</v>
       </c>
-      <c r="G144" t="s">
+      <c r="G145" t="s">
         <v>256</v>
-      </c>
-      <c r="H144" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>144</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="D145" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F145">
-        <v>5</v>
-      </c>
-      <c r="G145" t="s">
-        <v>258</v>
       </c>
       <c r="H145" t="s">
         <v>500</v>
@@ -7880,50 +8337,53 @@
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>145</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F146">
+        <v>5</v>
+      </c>
+      <c r="G146" t="s">
+        <v>258</v>
+      </c>
+      <c r="H146" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>146</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C147" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="D147" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E146" s="1" t="s">
+      <c r="E147" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G146" t="s">
+      <c r="G147" t="s">
         <v>285</v>
       </c>
-      <c r="H146" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
-        <v>146</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="D147" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G147" t="s">
-        <v>303</v>
-      </c>
       <c r="H147" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A148">
         <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
         <v>147</v>
@@ -7932,13 +8392,13 @@
         <v>134</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D148" s="4" t="s">
         <v>244</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="G148" t="s">
         <v>303</v>
@@ -7953,22 +8413,19 @@
         <v>148</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>27</v>
+        <v>244</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F149">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="G149" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="H149" t="s">
         <v>500</v>
@@ -7983,7 +8440,7 @@
         <v>26</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D150" s="4" t="s">
         <v>27</v>
@@ -8007,19 +8464,22 @@
         <v>150</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>317</v>
+        <v>427</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>220</v>
+        <v>30</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
       </c>
       <c r="G151" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="H151" t="s">
         <v>500</v>
@@ -8031,19 +8491,19 @@
         <v>151</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>243</v>
+        <v>317</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>31</v>
+        <v>220</v>
       </c>
       <c r="G152" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H152" t="s">
         <v>500</v>
@@ -8055,19 +8515,19 @@
         <v>152</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>452</v>
+        <v>243</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>219</v>
+        <v>23</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G153" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H153" t="s">
         <v>500</v>
@@ -8079,16 +8539,16 @@
         <v>153</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>428</v>
+        <v>452</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>183</v>
+        <v>40</v>
       </c>
       <c r="G154" t="s">
         <v>256</v>
@@ -8103,19 +8563,16 @@
         <v>154</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>10</v>
+        <v>182</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F155">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="G155" t="s">
         <v>256</v>
@@ -8130,19 +8587,19 @@
         <v>155</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F156">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G156" t="s">
         <v>256</v>
@@ -8160,7 +8617,7 @@
         <v>46</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D157" s="4" t="s">
         <v>13</v>
@@ -8184,19 +8641,22 @@
         <v>157</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>166</v>
+        <v>46</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>167</v>
+        <v>13</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>327</v>
+        <v>19</v>
+      </c>
+      <c r="F158">
+        <v>4</v>
       </c>
       <c r="G158" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
       <c r="H158" t="s">
         <v>500</v>
@@ -8208,19 +8668,19 @@
         <v>158</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>38</v>
+        <v>166</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>536</v>
+        <v>432</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>176</v>
+        <v>327</v>
       </c>
       <c r="G159" t="s">
-        <v>257</v>
+        <v>304</v>
       </c>
       <c r="H159" t="s">
         <v>500</v>
@@ -8237,10 +8697,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960A8748-E94B-4690-B759-C2243F7BF2D9}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8251,87 +8711,87 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="B1" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>589</v>
+        <v>627</v>
       </c>
       <c r="B2" t="s">
-        <v>590</v>
+        <v>628</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="B3" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="B4" t="s">
-        <v>615</v>
+        <v>584</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="B5" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="B6" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="B7" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B8" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="B9" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="B10" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="B11" t="s">
         <v>614</v>
@@ -8339,74 +8799,122 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>622</v>
+        <v>592</v>
       </c>
       <c r="B12" t="s">
-        <v>623</v>
+        <v>607</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="B13" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>600</v>
+        <v>617</v>
       </c>
       <c r="B14" t="s">
-        <v>601</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="B15" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="B16" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="B17" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="B18" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="B19" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="B20" t="s">
-        <v>613</v>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>605</v>
+      </c>
+      <c r="B21" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>629</v>
+      </c>
+      <c r="B22" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>630</v>
+      </c>
+      <c r="B23" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>631</v>
+      </c>
+      <c r="B24" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>632</v>
+      </c>
+      <c r="B25" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>633</v>
+      </c>
+      <c r="B26" t="s">
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -8422,7 +8930,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9292,295 +9800,1129 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFFD9FF-690D-4767-9960-BAF8E0E731BC}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="27" t="s">
         <v>550</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="27" t="s">
         <v>551</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="27" t="s">
         <v>552</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="27" t="s">
         <v>553</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="27" t="s">
         <v>554</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="27" t="s">
         <v>555</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="27" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+      <c r="A2" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="29" t="s">
+        <v>563</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>673</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29" t="s">
+        <v>674</v>
+      </c>
+      <c r="H2" s="39"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>563</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>563</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24" t="s">
+        <v>577</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>563</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>669</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>560</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="s">
+        <v>670</v>
+      </c>
+      <c r="H5" s="39"/>
+      <c r="I5" s="29"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>563</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>669</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>560</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29" t="s">
+        <v>671</v>
+      </c>
+      <c r="H6" s="39"/>
+      <c r="I6" s="29"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>563</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>669</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>560</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29" t="s">
+        <v>672</v>
+      </c>
+      <c r="H7" s="39"/>
+      <c r="I7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>563</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>564</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25" t="s">
+        <v>720</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>721</v>
+      </c>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>562</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25" t="s">
+        <v>559</v>
+      </c>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>557</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C10" s="29" t="s">
+        <v>675</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>676</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>677</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="29"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>684</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>685</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>701</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>680</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>681</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>701</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>682</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>683</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>701</v>
+      </c>
+      <c r="G13" s="29"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>637</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="I14" s="29"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>14</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>696</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>697</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>698</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="29"/>
+    </row>
+    <row r="16" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>15</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D16" s="36" t="s">
         <v>558</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E16" s="36" t="s">
+        <v>642</v>
+      </c>
+      <c r="F16" s="36" t="s">
         <v>561</v>
       </c>
-      <c r="F2" t="s">
-        <v>562</v>
-      </c>
-      <c r="H2" s="12" t="e" cm="1" vm="1">
-        <f t="array" ref="H2">_xlfn._xlws.PY(0,1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I2" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G16" s="28"/>
+      <c r="H16" s="37" t="s">
+        <v>638</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>16</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>648</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>649</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>650</v>
+      </c>
+      <c r="G17" s="29"/>
+      <c r="H17" s="40" t="s">
+        <v>651</v>
+      </c>
+      <c r="I17" s="29"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>17</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>678</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>679</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>677</v>
+      </c>
+      <c r="G18" s="29"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="29"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>18</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>699</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>700</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>702</v>
+      </c>
+      <c r="G19" s="29"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="29"/>
+    </row>
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>19</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="C20" s="36" t="s">
         <v>573</v>
       </c>
-      <c r="C3" t="s">
-        <v>563</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D20" s="36" t="s">
+        <v>558</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>667</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>666</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E21" t="s">
+        <v>646</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G21" s="29"/>
+      <c r="H21" s="41" t="s">
+        <v>647</v>
+      </c>
+      <c r="I21" s="29"/>
+    </row>
+    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>21</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>652</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E22" t="s">
+        <v>653</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>654</v>
+      </c>
+      <c r="G22" s="29"/>
+      <c r="H22" s="41" t="s">
+        <v>655</v>
+      </c>
+      <c r="I22" s="29"/>
+    </row>
+    <row r="23" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>22</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E23" t="s">
+        <v>635</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G23" s="29"/>
+      <c r="H23" s="35" t="s">
+        <v>636</v>
+      </c>
+      <c r="I23" s="29"/>
+    </row>
+    <row r="24" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A24" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>23</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>626</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>703</v>
+      </c>
+      <c r="G24" s="29"/>
+      <c r="H24" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="I24" s="29"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>24</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>710</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E25" t="s">
+        <v>711</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>25</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>712</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E26" t="s">
+        <v>713</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="29"/>
+    </row>
+    <row r="27" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A27" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>26</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E27" t="s">
+        <v>641</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G27" s="29"/>
+      <c r="H27" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="I27" s="29"/>
+    </row>
+    <row r="28" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A28" s="24">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>27</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>567</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>558</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>568</v>
+      </c>
+      <c r="G28" s="24"/>
+      <c r="H28" s="37" t="s">
+        <v>634</v>
+      </c>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A29" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>28</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>664</v>
+      </c>
+      <c r="D29" s="34"/>
+      <c r="E29" s="12" t="s">
+        <v>668</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>665</v>
+      </c>
+      <c r="G29" s="29"/>
+      <c r="H29" s="35" t="s">
+        <v>718</v>
+      </c>
+      <c r="I29" s="29"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>29</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>705</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E30" t="s">
+        <v>706</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="29"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>30</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>689</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E31" t="s">
+        <v>690</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>691</v>
+      </c>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="29"/>
+    </row>
+    <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>31</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>660</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E32" t="s">
+        <v>661</v>
+      </c>
+      <c r="F32" s="34" t="s">
+        <v>662</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="H32" s="35" t="s">
+        <v>663</v>
+      </c>
+      <c r="I32" s="29"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="34">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>32</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>531</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E33" t="s">
+        <v>688</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>650</v>
+      </c>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="29"/>
+    </row>
+    <row r="34" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A34" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>33</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E34" t="s">
+        <v>637</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>701</v>
+      </c>
+      <c r="G34" s="29"/>
+      <c r="H34" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="I34" s="29"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>34</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>558</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>565</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>566</v>
+      </c>
+      <c r="G35" s="25"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="31">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>35</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>570</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>558</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>704</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="33" t="s">
+        <v>640</v>
+      </c>
+      <c r="I36" s="25"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="34">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>36</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>694</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E37" t="s">
+        <v>695</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G37" s="29"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="29"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="34">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>37</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>709</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E38" t="s">
+        <v>639</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G38" s="29"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="29"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="34">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>38</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E39" t="s">
+        <v>708</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G39" s="29"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="29"/>
+    </row>
+    <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A40" s="31">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>39</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>656</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E40" t="s">
+        <v>657</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>658</v>
+      </c>
+      <c r="G40" s="29"/>
+      <c r="H40" s="35" t="s">
+        <v>659</v>
+      </c>
+      <c r="I40" s="29"/>
+    </row>
+    <row r="41" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A41" s="31">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>40</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E41" t="s">
+        <v>639</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="G41" s="29"/>
+      <c r="H41" s="35" t="s">
+        <v>717</v>
+      </c>
+      <c r="I41" s="29"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="34">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>41</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="E42" t="s">
+        <v>686</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>687</v>
+      </c>
+      <c r="G42" s="29"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="29"/>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="29">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>42</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>693</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>702</v>
+      </c>
+      <c r="G43" s="29"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="29"/>
+    </row>
+    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>43</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E44" t="s">
+        <v>643</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>644</v>
+      </c>
+      <c r="G44" s="29"/>
+      <c r="H44" s="35" t="s">
+        <v>645</v>
+      </c>
+      <c r="I44" s="29"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>44</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="D45" s="25" t="s">
         <v>560</v>
       </c>
-      <c r="G3" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>565</v>
-      </c>
-      <c r="C5" t="s">
-        <v>566</v>
-      </c>
-      <c r="D5" t="s">
-        <v>560</v>
-      </c>
-      <c r="G5" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>565</v>
-      </c>
-      <c r="C6" t="s">
-        <v>566</v>
-      </c>
-      <c r="D6" t="s">
-        <v>560</v>
-      </c>
-      <c r="G6" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>557</v>
-      </c>
-      <c r="C7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" t="s">
-        <v>558</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>569</v>
-      </c>
-      <c r="F7" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>557</v>
-      </c>
-      <c r="C8" t="s">
-        <v>571</v>
-      </c>
-      <c r="D8" t="s">
-        <v>558</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>576</v>
-      </c>
-      <c r="F8" t="s">
-        <v>572</v>
-      </c>
-      <c r="H8" s="12" t="e" cm="1" vm="2">
-        <f t="array" ref="H8">_xlfn._xlws.PY(1,1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>557</v>
-      </c>
-      <c r="C9" t="s">
-        <v>574</v>
-      </c>
-      <c r="D9" t="s">
-        <v>558</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>575</v>
-      </c>
-      <c r="F9" t="s">
-        <v>577</v>
-      </c>
-      <c r="H9" t="e" cm="1" vm="3">
-        <f t="array" ref="H9">_xlfn._xlws.PY(2,1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>557</v>
-      </c>
-      <c r="C10" t="s">
-        <v>578</v>
-      </c>
-      <c r="D10" t="s">
-        <v>558</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>580</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E45" s="31"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>565</v>
-      </c>
-      <c r="C11" t="s">
-        <v>581</v>
-      </c>
-      <c r="D11" t="s">
-        <v>560</v>
-      </c>
-      <c r="G11" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>565</v>
-      </c>
-      <c r="C12" t="s">
-        <v>583</v>
-      </c>
-      <c r="D12" t="s">
-        <v>560</v>
-      </c>
-      <c r="G12" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>585</v>
-      </c>
-      <c r="C13" t="s">
-        <v>585</v>
-      </c>
-      <c r="D13" t="s">
-        <v>560</v>
-      </c>
-      <c r="G13" t="s">
-        <v>586</v>
-      </c>
+      <c r="H45" s="31"/>
+      <c r="I45" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -9633,7 +10975,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>545</v>
@@ -9657,42 +10999,42 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: atualizar kit de medicamentos com novas prescrições e ajustes nas prioridades
</commit_message>
<xml_diff>
--- a/script-excel-para-json/input/prescricoes.xlsx
+++ b/script-excel-para-json/input/prescricoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1AC289667D0E8CCD/Documentos/Saúde/Prescrições/Prescrição_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2396" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EFAAB7E-B676-4E43-8038-6689DBE959E8}"/>
+  <xr:revisionPtr revIDLastSave="2504" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A94DD4C-A85E-48F1-BC1C-8944F5847901}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="2" activeTab="7" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" firstSheet="2" activeTab="7" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
   </bookViews>
   <sheets>
     <sheet name="Para_casa" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="748">
   <si>
     <t>NomeBusca</t>
   </si>
@@ -2269,13 +2269,6 @@
     <t>Sinais vitais</t>
   </si>
   <si>
-    <t>25 mg Comp;
-50 mg Comp</t>
-  </si>
-  <si>
-    <t>mg; Comp</t>
-  </si>
-  <si>
     <t>Fentanil</t>
   </si>
   <si>
@@ -2478,21 +2471,6 @@
   </si>
   <si>
     <t>Noite</t>
-  </si>
-  <si>
-    <t>[
-	{
-		"nome": "Fentanil 10 mcg BIC",
-		"texto": "Fentanil 50 mcg/ml, 20 ml, BIC, vazão ACM. Concentração: 10 mcg/ml",
-		"componentes":	[
-			{
-				"item": "Glicose à 5%",
-				"dose": "80",
-				"unidade": "ml"
-			}
-					]
-	}
-]</t>
   </si>
   <si>
     <t>25 mg/ml Amp 3</t>
@@ -2708,9 +2686,6 @@
     <t>Controle glicêmico</t>
   </si>
   <si>
-    <t>Controles glicêmicos a cada 4/4h</t>
-  </si>
-  <si>
     <t>Acído acetilsalicílico</t>
   </si>
   <si>
@@ -2916,6 +2891,383 @@
 	{
 		"nome": "SSVV 6/6h",
 		"texto": "Aferir sinais vitais de 6 em 6 horas"
+	}
+]</t>
+  </si>
+  <si>
+    <t>Dor osteomuscular</t>
+  </si>
+  <si>
+    <t>Sistema musculo esquelético</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso oral
+1 - Dipirona 500 mg _____ 1 caixa
+Tomar 1 comprimido de 6 em 6 horas se dor ou febre
+Obs.: Pode tomar até 2 comprimidos de 6 em 6 horas
+Obs. 2: Se não melhora somente com a dipirona, continue tomando-a junto com o anti-inflamatório abaixo
+1 - Naproxeno 500 mg _____ 1 caixa
+Tomar 1 comprimido de 12 em 12 horas por até 5 dias
+1 - Ciclobenzaprina 10 mg _____ 1 caixa
+Tomar 1 comprimido por dia à noite por 7 dias
+</t>
+  </si>
+  <si>
+    <t>50 mg/ml Amp 2 ml</t>
+  </si>
+  <si>
+    <t>Sacarato de hidroxido férrico</t>
+  </si>
+  <si>
+    <t>20 mg/ml Amp 5 ml</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Sacarato de hidroxido férrico 200 mg agora",
+        "texto": "Sacarato de hidroxido férrico 20 mg/ml, 5 ml (1 ampola), EV, agora",
+        "componentes": [
+            {
+                "item": "Cloreto de sódio à 0,9%",
+                "dose": "100",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "infundir em 1 hora"
+    }   
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Sulfato de magnésio 20%, 2g, agora",
+        "texto": "Sulfato de magnésio 20%, 10 ml (1 ampola), EV, agora",
+        "componentes": [
+            {
+                "item": "Cloreto de sódio à 0,9%",
+                "dose": "100",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "Infundir em 30 minutos"
+    }   
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Tramadol 100 mg agora",
+        "texto": "Tramadol 100 mg/ml, 2 ml (1 ampola), EV, agora",
+        "componentes": [
+            {
+                "item": "Cloreto de sódio à 0,9%",
+                "dose": "100",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "Infundir em 30-60 minutos"
+    },
+    {
+        "nome": "Tramadol 100 mg 6/6h se necessário",
+        "texto": "Tramadol 100 mg/ml, 2 ml (1 ampola), 6/6h, se dor",
+        "componentes": [
+            {
+                "item": "Cloreto de sódio à 0,9%",
+                "dose": "100",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "Infundir em 30-60 minutos"
+    }
+   ]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Norepinefrina 64 mcg/ml BIC",
+        "texto": "Norepinefrina 1 mg/ml, 16 ml, BIC, vazão ACM. Concentração: 64 mcg/ml",
+        "componentes": [
+            {
+                "item": "SG 5%",
+                "dose": "234",
+                "unidade": "ml"
+            }
+        ]
+    },
+    {
+        "nome": "Norepinefrina 160 mcg/ml BIC",
+        "texto": "Norepinefrina 1 mg/ml, 16 ml, BIC, vazão ACM. Concentração: 160 mcg/ml",
+        "componentes": [
+            {
+                "item": "SG 5%",
+                "dose": "84",
+                "unidade": "ml"
+            }
+        ]
+    },
+    {
+        "nome": "Norepinefrina 200 mcg/ml BIC",
+        "texto": "Norepinefrina 1 mg/ml, 20 ml, BIC, vazão ACM. Concentração: 200 mcg/ml",
+        "componentes": [
+            {
+                "item": "SG 5%",
+                "dose": "80",
+                "unidade": "ml"
+            }
+        ]
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Nitroprussiato 200 mcg/ml BIC",
+        "texto": "Nitroprussiato 25 mg/ml, 2 ml, BIC, vazão ACM. Concentração: 200 mcg/ml",
+        "componentes": [
+            {
+                "item": "SG 5%",
+                "dose": "248",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "Em equipo para fotoproteção"
+    }
+]</t>
+  </si>
+  <si>
+    <t>Nitroglicerina</t>
+  </si>
+  <si>
+    <t>5 mg/ml Amp 5 ml;
+5 mg/ml Amp 10ml</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Nitroglicerina 200 mcg/ml BIC",
+        "texto": "Nitroprussiato 25 mg/ml, 10 ml, BIC, vazão ACM. Concentração: 200 mcg/ml",
+        "componentes": [
+            {
+                "item": "SF 0,9% ou SG 5%",
+                "dose": "240",
+                "unidade": "ml"
+            }
+        ]
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Morfina 2 mg agora",
+        "texto": "Morfina 10 mg/ml, 1 ml (1 ampola), EV, bolus, agora",
+        "componentes": [
+            {
+                "item": "ABD",
+                "dose": "9",
+                "unidade": "ml"
+            }
+        ]
+    },
+{
+        "nome": "Morfina 1 mg/ml BIC",
+        "texto": "Morfina 10 mg/ml, 10 ml (10 ampolas), EV, BIC, vazão ACM. Concentração: 1 mg/ml",
+        "componentes": [
+            {
+                "item": "SG 5%",
+                "dose": "90",
+                "unidade": "ml"
+            }
+        ]
+    }
+]</t>
+  </si>
+  <si>
+    <t>25 mg Comp;
+50 mg Comp;
+1 mg/ml Amp 5 ml</t>
+  </si>
+  <si>
+    <t>mg; ml; Comp; ampola</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Fentanil 10 mcg/ml BIC",
+		"texto": "Fentanil 50 mcg/ml, 20 ml, BIC, vazão ACM. Concentração: 10 mcg/ml",
+		"componentes":	[
+			{
+				"item": "Glicose à 5%",
+				"dose": "80",
+				"unidade": "ml"
+			}
+					]
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Dopamina 1000 mcg/ml BIC (100 ml)",
+		"texto": "Dopamina 5 mg/ml, 20 ml, BIC, vazão ACM. Concentração: 1000 mcg/ml",
+		"componentes":	[
+			{
+				"item": "SF 0,9% ou SG 5%",
+				"dose": "80",
+				"unidade": "ml"
+			}
+					]
+	},
+	{
+		"nome": "Dopamina 1000 mcg/ml BIC (100 ml)",
+		"texto": "Dopamina 5 mg/ml, 50 ml (5 ampolas), BIC, vazão ACM. Concentração: 1000 mcg/ml",
+		"componentes":	[
+			{
+				"item": "SF 0,9% ou SG 5%",
+				"dose": "200",
+				"unidade": "ml"
+			}
+					]
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Dobutamina 4000 mcg/ml BIC",
+		"texto": "Dobutamina 250 mg/20 ml, 80 ml, BIC, vazão ACM. Concentração: 4000 mcg/ml",
+		"componentes":	[
+			{
+				"item": "SF 0,9% ou SG 5%",
+				"dose": "170",
+				"unidade": "ml"
+			}
+					]
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Cloreto de sódio à 3% BIC",
+		"texto": "Cloreto de sódio 20%, 55 ml, BIC, vazão ACM. Concentração: 3%",
+		"componentes":	[
+			{
+				"item": "SF 0,9%",
+				"dose": "445",
+				"unidade": "ml"
+			}
+					]
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Cloreto de potássio 19,1% 75 mEq/L BIC",
+		"texto": "Cloreto de potássio 19,1%, 15 ml, BIC, infundir em 3 horas. Concentração: 75 mEq/L",
+		"componentes":	[
+			{
+				"item": "SF 0,9%",
+				"dose": "485",
+				"unidade": "ml"
+			}
+					],
+		"observacao": "Pode infundir em via periférica"
+	},
+	{
+		"nome": "Cloreto de potássio 19,1% 100 mEq/L BIC",
+		"texto": "Cloreto de potássio 19,1%, 10 ml, BIC, infundir em 2 horas. Concentração: 100 mEq/L",
+		"componentes":	[
+			{
+				"item": "SF 0,9%",
+				"dose": "240",
+				"unidade": "ml"
+			}
+					],
+		"observacao": "Infundir em veia central"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Clopidogrel  300 mg agora",
+		"texto": "Clopidogrel 75 mg, 300 mg (4 comprimidos), VO, agora"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "AAS  300 mg agora",
+		"texto": "Acido acetilsalicílico 100 mg, 300 mg (3 comprimidos), VO, agora"
+	}
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Amiodarona 150 mg agora",
+        "texto": "Amiodarona 50 mg/ml, 3 ml (1 ampola), EV, agora",
+        "componentes": [
+            {
+                "item": "Glicose à 5%",
+                "dose": "100",
+                "unidade": "ml"
+            }
+        ],
+        "observacao": "Infundir em 30 minutos"
+    },
+    {
+        "nome": "Amiodarona 3,6 mg/ml BIC",
+        "texto": "Amiodarona 50 mg/ml, 18 ml (6 ampola), EV, BIC, vazão ACM. Concentração: 3,6 mg/ml",
+        "componentes": [
+            {
+                "item": "Glicose à 5%",
+                "dose": "234",
+                "unidade": "ml"
+            }
+        ]
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "nome": "Metoprolol 5 mg agora",
+        "texto": "Metoprolol 1 mg/ml, 5 ml (1 ampola) em 5 ml de ABD, EV, lento, agora"
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "HGT 4/4h",
+		"texto": "Controle glicêmico 4 em 4 horas"
+	},
+	{
+		"nome": "HGT 1/1h",
+		"texto": "Controle glicêmico 1 em 1 hora"
+	}
+]</t>
+  </si>
+  <si>
+    <t>Manter grades elevadas</t>
+  </si>
+  <si>
+    <t>Prevenção de quedas</t>
+  </si>
+  <si>
+    <t>[
+	{
+		"nome": "Salbutamol 4 jatos com espaçador 20/20 min",
+		"texto": "Salbutamol 100 mcg aerossol, 4 jatos a cada 20 minutos por 1 hora, via inalatória, agora",
+		"observação": "Usar espaçador"
+	},
+	{
+		"nome": "Salbutamol 6 jatos 20/20 min",
+		"texto": "Salbutamol 100 mcg aerossol, 6 jatos a cada 20 minutos por 1 hora, via inalatória, agora"
 	}
 ]</t>
   </si>
@@ -3058,7 +3410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3116,6 +3468,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3146,6 +3501,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3866,11 +4227,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}" name="Tabela8" displayName="Tabela8" ref="A1:E6" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A1:E6" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}" name="Tabela8" displayName="Tabela8" ref="A1:E7" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A1:E7" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C07F2220-FEC5-4C0B-AB14-F80860FCB6A0}" name="ID_Item" dataDxfId="37">
-      <calculatedColumnFormula>ROW() - ROW(Tabela5[[#Headers],[ID_Item]])</calculatedColumnFormula>
+      <calculatedColumnFormula>ROW() - ROW(Tabela8[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{F6AB2AED-7D50-4A14-A3D8-3D697CD7C3E6}" name="NomeBusca" dataDxfId="36"/>
     <tableColumn id="3" xr3:uid="{24DCE466-5828-477A-94D8-8B94F125CA52}" name="ConteudoTexto" dataDxfId="35"/>
@@ -3931,10 +4292,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4B1D6705-EEC4-44EF-9410-0F0CC297D1AF}" name="Tabela11" displayName="Tabela11" ref="A1:I45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A1:I45" xr:uid="{4B1D6705-EEC4-44EF-9410-0F0CC297D1AF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I45">
-    <sortCondition ref="B1:B45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4B1D6705-EEC4-44EF-9410-0F0CC297D1AF}" name="Tabela11" displayName="Tabela11" ref="A1:I49" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A1:I49" xr:uid="{4B1D6705-EEC4-44EF-9410-0F0CC297D1AF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I49">
+    <sortCondition ref="B1:B49"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{301BA950-EFFF-4FE5-9DB9-5861171DCD47}" name="ID" dataDxfId="7">
@@ -4284,7 +4645,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:V159"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
@@ -8711,210 +9072,210 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B2" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B3" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B7" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B9" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B10" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B11" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B13" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B14" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B15" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B16" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B17" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B18" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B19" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B20" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B21" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B22" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B23" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B24" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B25" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B26" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -9243,18 +9604,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1623D2DD-2AAF-46F4-A228-AB579D2CF3FD}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="104.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9277,6 +9638,7 @@
     </row>
     <row r="2" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
+        <f>ROW() - ROW(Tabela8[[#Headers],[ID_Item]])</f>
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -9294,6 +9656,7 @@
     </row>
     <row r="3" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
+        <f>ROW() - ROW(Tabela8[[#Headers],[ID_Item]])</f>
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -9306,11 +9669,12 @@
         <v>272</v>
       </c>
       <c r="E3" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
+        <f>ROW() - ROW(Tabela8[[#Headers],[ID_Item]])</f>
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -9323,11 +9687,12 @@
         <v>274</v>
       </c>
       <c r="E4" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
+        <f>ROW() - ROW(Tabela8[[#Headers],[ID_Item]])</f>
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -9345,6 +9710,7 @@
     </row>
     <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
+        <f>ROW() - ROW(Tabela8[[#Headers],[ID_Item]])</f>
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -9357,14 +9723,29 @@
         <v>275</v>
       </c>
       <c r="E6" s="13">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <f>ROW() - ROW(Tabela8[[#Headers],[ID_Item]])</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>718</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>720</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>719</v>
+      </c>
+      <c r="E7" s="43">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <ignoredErrors>
-    <ignoredError sqref="A3:A5" calculatedColumn="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -9800,10 +10181,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFFD9FF-690D-4767-9960-BAF8E0E731BC}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9820,1103 +10201,1233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>549</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>550</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="28" t="s">
         <v>551</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="28" t="s">
         <v>552</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="28" t="s">
         <v>553</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="28" t="s">
         <v>554</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="28" t="s">
         <v>555</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="28" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>563</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>673</v>
-      </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29" t="s">
-        <v>674</v>
-      </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="29"/>
+      <c r="C2" s="30" t="s">
+        <v>670</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30" t="s">
+        <v>670</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>744</v>
+      </c>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>563</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>574</v>
-      </c>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="26" t="s">
+        <v>572</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>560</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25" t="s">
-        <v>575</v>
-      </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26" t="s">
+        <v>573</v>
+      </c>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
+      <c r="A4" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="30" t="s">
         <v>563</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="30" t="s">
+        <v>746</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24" t="s">
-        <v>577</v>
-      </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30" t="s">
+        <v>745</v>
+      </c>
+      <c r="H4" s="40"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>4</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>563</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>669</v>
-      </c>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="24" t="s">
+        <v>574</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>560</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29" t="s">
-        <v>670</v>
-      </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="29"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24" t="s">
+        <v>575</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>5</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="26" t="s">
         <v>563</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>669</v>
-      </c>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29" t="s">
-        <v>671</v>
-      </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="29"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30" t="s">
+        <v>667</v>
+      </c>
+      <c r="H6" s="40"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
+      <c r="A7" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="26" t="s">
         <v>563</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>669</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29" t="s">
-        <v>672</v>
-      </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="29"/>
-    </row>
-    <row r="8" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="E7" s="26"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30" t="s">
+        <v>668</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>7</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="30" t="s">
         <v>563</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>564</v>
-      </c>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25" t="s">
-        <v>720</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>721</v>
-      </c>
-      <c r="I8" s="25"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="E8" s="26"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="H8" s="40"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>8</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>569</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>562</v>
-      </c>
-      <c r="D9" s="25" t="s">
+      <c r="B9" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>560</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25" t="s">
-        <v>559</v>
-      </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26" t="s">
+        <v>716</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>717</v>
+      </c>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>9</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>557</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>675</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>558</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>676</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>677</v>
-      </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="29"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="B10" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>562</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>560</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>10</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>684</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="C11" s="30" t="s">
+        <v>671</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>558</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>685</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>701</v>
-      </c>
-      <c r="G11" s="29"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="29"/>
+      <c r="E11" s="26" t="s">
+        <v>672</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="41" t="s">
+        <v>741</v>
+      </c>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
+      <c r="A12" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>11</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="30" t="s">
         <v>680</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="30" t="s">
         <v>558</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="32" t="s">
         <v>681</v>
       </c>
-      <c r="F12" s="29" t="s">
-        <v>701</v>
-      </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="29"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="F12" s="30" t="s">
+        <v>697</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>12</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>682</v>
-      </c>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="30" t="s">
+        <v>676</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>558</v>
       </c>
-      <c r="E13" s="33" t="s">
-        <v>683</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>701</v>
-      </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A14" s="25">
+      <c r="E13" s="32" t="s">
+        <v>677</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>697</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="38" t="s">
+        <v>742</v>
+      </c>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>13</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" s="34" t="s">
+      <c r="C14" s="35" t="s">
+        <v>678</v>
+      </c>
+      <c r="D14" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>637</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="26" t="s">
-        <v>714</v>
-      </c>
-      <c r="I14" s="29"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
+      <c r="E14" s="34" t="s">
+        <v>679</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="15" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>14</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>696</v>
-      </c>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="32" t="s">
+        <v>634</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>697</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>698</v>
-      </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="29"/>
-    </row>
-    <row r="16" spans="1:9" ht="390" x14ac:dyDescent="0.25">
-      <c r="A16" s="24">
+      <c r="G15" s="30"/>
+      <c r="H15" s="27" t="s">
+        <v>710</v>
+      </c>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>15</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="36" t="s">
+      <c r="C16" s="35" t="s">
+        <v>692</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E16" s="36" t="s">
-        <v>642</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>561</v>
-      </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="37" t="s">
-        <v>638</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="25">
+      <c r="E16" s="32" t="s">
+        <v>693</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>694</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>16</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>648</v>
-      </c>
-      <c r="D17" s="34" t="s">
+      <c r="C17" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="E17" s="31" t="s">
-        <v>649</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>650</v>
+      <c r="E17" s="37" t="s">
+        <v>639</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>561</v>
       </c>
       <c r="G17" s="29"/>
-      <c r="H17" s="40" t="s">
-        <v>651</v>
-      </c>
-      <c r="I17" s="29"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+      <c r="H17" s="25" t="s">
+        <v>635</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>17</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C18" s="34" t="s">
-        <v>678</v>
-      </c>
-      <c r="D18" s="34" t="s">
+      <c r="C18" s="35" t="s">
+        <v>645</v>
+      </c>
+      <c r="D18" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E18" s="31" t="s">
-        <v>679</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>677</v>
-      </c>
-      <c r="G18" s="29"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="29"/>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="E18" s="32" t="s">
+        <v>646</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>647</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="41" t="s">
+        <v>648</v>
+      </c>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>18</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C19" s="34" t="s">
-        <v>699</v>
-      </c>
-      <c r="D19" s="34" t="s">
+      <c r="C19" s="35" t="s">
+        <v>674</v>
+      </c>
+      <c r="D19" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>700</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>702</v>
-      </c>
-      <c r="G19" s="29"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="29"/>
-    </row>
-    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="24">
+      <c r="E19" s="32" t="s">
+        <v>675</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>673</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="42" t="s">
+        <v>740</v>
+      </c>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+      <c r="A20" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>19</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C20" s="36" t="s">
-        <v>573</v>
-      </c>
-      <c r="D20" s="36" t="s">
+      <c r="C20" s="35" t="s">
+        <v>695</v>
+      </c>
+      <c r="D20" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E20" s="38" t="s">
-        <v>667</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>666</v>
-      </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="24"/>
-    </row>
-    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="25">
+      <c r="E20" s="34" t="s">
+        <v>696</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>698</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="38" t="s">
+        <v>739</v>
+      </c>
+      <c r="I20" s="30"/>
+    </row>
+    <row r="21" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>20</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="C21" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="D21" s="34" t="s">
+      <c r="C21" s="37" t="s">
+        <v>571</v>
+      </c>
+      <c r="D21" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="E21" t="s">
-        <v>646</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="41" t="s">
-        <v>647</v>
-      </c>
-      <c r="I21" s="29"/>
-    </row>
-    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="25">
+      <c r="E21" s="39" t="s">
+        <v>664</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>663</v>
+      </c>
+      <c r="G21" s="24"/>
+      <c r="H21" s="38" t="s">
+        <v>738</v>
+      </c>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>21</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C22" s="34" t="s">
-        <v>652</v>
-      </c>
-      <c r="D22" s="34" t="s">
+      <c r="C22" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E22" t="s">
-        <v>653</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>654</v>
-      </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="41" t="s">
-        <v>655</v>
-      </c>
-      <c r="I22" s="29"/>
-    </row>
-    <row r="23" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="25">
+        <v>643</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="42" t="s">
+        <v>644</v>
+      </c>
+      <c r="I22" s="30"/>
+    </row>
+    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>22</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="34" t="s">
+      <c r="C23" s="35" t="s">
+        <v>649</v>
+      </c>
+      <c r="D23" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E23" t="s">
-        <v>635</v>
-      </c>
-      <c r="F23" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="35" t="s">
-        <v>636</v>
-      </c>
-      <c r="I23" s="29"/>
-    </row>
-    <row r="24" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A24" s="25">
+        <v>650</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>651</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="42" t="s">
+        <v>652</v>
+      </c>
+      <c r="I23" s="30"/>
+    </row>
+    <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>23</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="34" t="s">
+      <c r="C24" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E24" s="33" t="s">
-        <v>626</v>
-      </c>
-      <c r="F24" s="34" t="s">
-        <v>703</v>
-      </c>
-      <c r="G24" s="29"/>
-      <c r="H24" s="33" t="s">
-        <v>715</v>
-      </c>
-      <c r="I24" s="29"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="E24" t="s">
+        <v>632</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="42" t="s">
+        <v>633</v>
+      </c>
+      <c r="I24" s="30"/>
+    </row>
+    <row r="25" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>24</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="C25" s="34" t="s">
-        <v>710</v>
-      </c>
-      <c r="D25" s="34" t="s">
+      <c r="C25" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="34" t="s">
+        <v>624</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>699</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="34" t="s">
         <v>711</v>
       </c>
-      <c r="F25" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="29"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
+      <c r="I25" s="30"/>
+    </row>
+    <row r="26" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A26" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>25</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="C26" s="34" t="s">
-        <v>712</v>
-      </c>
-      <c r="D26" s="34" t="s">
+      <c r="C26" s="35" t="s">
+        <v>706</v>
+      </c>
+      <c r="D26" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E26" t="s">
-        <v>713</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="29"/>
-    </row>
-    <row r="27" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A27" s="25">
+        <v>707</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="38" t="s">
+        <v>737</v>
+      </c>
+      <c r="I26" s="30"/>
+    </row>
+    <row r="27" spans="1:9" ht="360" x14ac:dyDescent="0.25">
+      <c r="A27" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>26</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C27" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="34" t="s">
+      <c r="C27" s="35" t="s">
+        <v>708</v>
+      </c>
+      <c r="D27" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E27" t="s">
-        <v>641</v>
-      </c>
-      <c r="F27" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G27" s="29"/>
-      <c r="H27" s="33" t="s">
-        <v>716</v>
-      </c>
-      <c r="I27" s="29"/>
-    </row>
-    <row r="28" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A28" s="24">
+        <v>709</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="38" t="s">
+        <v>736</v>
+      </c>
+      <c r="I27" s="30"/>
+    </row>
+    <row r="28" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A28" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>27</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C28" s="36" t="s">
-        <v>567</v>
-      </c>
-      <c r="D28" s="36" t="s">
+      <c r="C28" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E28" s="37" t="s">
-        <v>572</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>568</v>
-      </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="I28" s="24"/>
-    </row>
-    <row r="29" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A29" s="25">
+      <c r="E28" t="s">
+        <v>638</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="34" t="s">
+        <v>712</v>
+      </c>
+      <c r="I28" s="30"/>
+    </row>
+    <row r="29" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A29" s="24">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>28</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="C29" s="34" t="s">
-        <v>664</v>
-      </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="12" t="s">
-        <v>668</v>
-      </c>
-      <c r="F29" s="34" t="s">
-        <v>665</v>
-      </c>
-      <c r="G29" s="29"/>
-      <c r="H29" s="35" t="s">
-        <v>718</v>
-      </c>
-      <c r="I29" s="29"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
+      <c r="C29" s="37" t="s">
+        <v>565</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>558</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>570</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="G29" s="24"/>
+      <c r="H29" s="38" t="s">
+        <v>735</v>
+      </c>
+      <c r="I29" s="24"/>
+    </row>
+    <row r="30" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A30" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>29</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C30" s="34" t="s">
-        <v>705</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>558</v>
-      </c>
-      <c r="E30" t="s">
-        <v>706</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="29"/>
+      <c r="C30" s="35" t="s">
+        <v>661</v>
+      </c>
+      <c r="D30" s="35"/>
+      <c r="E30" s="12" t="s">
+        <v>665</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="G30" s="30"/>
+      <c r="H30" s="36" t="s">
+        <v>714</v>
+      </c>
+      <c r="I30" s="30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
+      <c r="A31" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>30</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>689</v>
-      </c>
-      <c r="D31" s="29" t="s">
+      <c r="C31" s="30" t="s">
+        <v>701</v>
+      </c>
+      <c r="D31" s="30" t="s">
         <v>558</v>
       </c>
       <c r="E31" t="s">
-        <v>690</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>691</v>
-      </c>
-      <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="29"/>
-    </row>
-    <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="31">
+        <v>702</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>697</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="30"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="35">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>31</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C32" s="34" t="s">
-        <v>660</v>
-      </c>
-      <c r="D32" s="34" t="s">
+      <c r="C32" s="35" t="s">
+        <v>685</v>
+      </c>
+      <c r="D32" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E32" t="s">
-        <v>661</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>662</v>
-      </c>
-      <c r="G32" s="29"/>
-      <c r="H32" s="35" t="s">
-        <v>663</v>
-      </c>
-      <c r="I32" s="29"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="34">
+        <v>686</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>687</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="30"/>
+    </row>
+    <row r="33" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="32">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>32</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C33" s="34" t="s">
-        <v>531</v>
-      </c>
-      <c r="D33" s="34" t="s">
+      <c r="C33" s="35" t="s">
+        <v>657</v>
+      </c>
+      <c r="D33" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E33" t="s">
-        <v>688</v>
-      </c>
-      <c r="F33" s="34" t="s">
-        <v>650</v>
-      </c>
-      <c r="G33" s="29"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="29"/>
-    </row>
-    <row r="34" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A34" s="25">
+        <v>658</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>659</v>
+      </c>
+      <c r="G33" s="30"/>
+      <c r="H33" s="36" t="s">
+        <v>660</v>
+      </c>
+      <c r="I33" s="30"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>33</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C34" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="29" t="s">
+      <c r="C34" s="30" t="s">
+        <v>531</v>
+      </c>
+      <c r="D34" s="30" t="s">
         <v>558</v>
       </c>
       <c r="E34" t="s">
-        <v>637</v>
-      </c>
-      <c r="F34" s="29" t="s">
-        <v>701</v>
-      </c>
-      <c r="G34" s="29"/>
-      <c r="H34" s="33" t="s">
-        <v>719</v>
-      </c>
-      <c r="I34" s="29"/>
-    </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="31">
+        <v>684</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>647</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="30"/>
+    </row>
+    <row r="35" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A35" s="32">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>34</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C35" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="D35" s="31" t="s">
+      <c r="C35" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E35" s="33" t="s">
-        <v>565</v>
-      </c>
-      <c r="F35" s="31" t="s">
-        <v>566</v>
-      </c>
-      <c r="G35" s="25"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="25"/>
-    </row>
-    <row r="36" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="31">
+      <c r="E35" t="s">
+        <v>634</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G35" s="30"/>
+      <c r="H35" s="34" t="s">
+        <v>715</v>
+      </c>
+      <c r="I35" s="30"/>
+    </row>
+    <row r="36" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="32">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>35</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="32" t="s">
         <v>557</v>
       </c>
-      <c r="C36" s="31" t="s">
-        <v>570</v>
-      </c>
-      <c r="D36" s="31" t="s">
+      <c r="C36" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="32" t="s">
         <v>558</v>
       </c>
-      <c r="E36" s="33" t="s">
-        <v>571</v>
-      </c>
-      <c r="F36" s="31" t="s">
-        <v>704</v>
-      </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="33" t="s">
-        <v>640</v>
-      </c>
-      <c r="I36" s="25"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="34">
+      <c r="E36" s="34" t="s">
+        <v>733</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>734</v>
+      </c>
+      <c r="G36" s="26"/>
+      <c r="H36" s="34" t="s">
+        <v>743</v>
+      </c>
+      <c r="I36" s="26"/>
+    </row>
+    <row r="37" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="32">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>36</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="32" t="s">
         <v>557</v>
       </c>
-      <c r="C37" s="34" t="s">
-        <v>694</v>
-      </c>
-      <c r="D37" s="34" t="s">
+      <c r="C37" s="32" t="s">
+        <v>568</v>
+      </c>
+      <c r="D37" s="32" t="s">
         <v>558</v>
       </c>
-      <c r="E37" t="s">
-        <v>695</v>
-      </c>
-      <c r="F37" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="29"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="34">
+      <c r="E37" s="34" t="s">
+        <v>569</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>700</v>
+      </c>
+      <c r="G37" s="26"/>
+      <c r="H37" s="34" t="s">
+        <v>637</v>
+      </c>
+      <c r="I37" s="26"/>
+    </row>
+    <row r="38" spans="1:9" ht="360" x14ac:dyDescent="0.25">
+      <c r="A38" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>37</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="C38" s="34" t="s">
-        <v>709</v>
-      </c>
-      <c r="D38" s="34" t="s">
+      <c r="C38" s="30" t="s">
+        <v>690</v>
+      </c>
+      <c r="D38" s="30" t="s">
         <v>558</v>
       </c>
       <c r="E38" t="s">
-        <v>639</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G38" s="29"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="29"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="34">
+        <v>691</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>697</v>
+      </c>
+      <c r="G38" s="30"/>
+      <c r="H38" s="38" t="s">
+        <v>732</v>
+      </c>
+      <c r="I38" s="30"/>
+    </row>
+    <row r="39" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A39" s="35">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>38</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C39" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="D39" s="34" t="s">
+      <c r="C39" s="35" t="s">
+        <v>729</v>
+      </c>
+      <c r="D39" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E39" t="s">
-        <v>708</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G39" s="29"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="29"/>
-    </row>
-    <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="31">
+      <c r="E39" s="12" t="s">
+        <v>730</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G39" s="30"/>
+      <c r="H39" s="34" t="s">
+        <v>731</v>
+      </c>
+      <c r="I39" s="30"/>
+    </row>
+    <row r="40" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A40" s="35">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>39</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>656</v>
-      </c>
-      <c r="D40" s="34" t="s">
+      <c r="C40" s="35" t="s">
+        <v>705</v>
+      </c>
+      <c r="D40" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E40" t="s">
-        <v>657</v>
-      </c>
-      <c r="F40" s="34" t="s">
-        <v>658</v>
-      </c>
-      <c r="G40" s="29"/>
-      <c r="H40" s="35" t="s">
-        <v>659</v>
-      </c>
-      <c r="I40" s="29"/>
-    </row>
-    <row r="41" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A41" s="31">
+        <v>636</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G40" s="30"/>
+      <c r="H40" s="34" t="s">
+        <v>728</v>
+      </c>
+      <c r="I40" s="30"/>
+    </row>
+    <row r="41" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="35">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>40</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C41" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="D41" s="34" t="s">
+      <c r="C41" s="35" t="s">
+        <v>703</v>
+      </c>
+      <c r="D41" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E41" t="s">
-        <v>639</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>701</v>
-      </c>
-      <c r="G41" s="29"/>
-      <c r="H41" s="35" t="s">
-        <v>717</v>
-      </c>
-      <c r="I41" s="29"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="34">
+        <v>704</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G41" s="30"/>
+      <c r="H41" s="34" t="s">
+        <v>727</v>
+      </c>
+      <c r="I41" s="30"/>
+    </row>
+    <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="32">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>41</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C42" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="34" t="s">
+      <c r="C42" s="35" t="s">
+        <v>653</v>
+      </c>
+      <c r="D42" s="35" t="s">
         <v>558</v>
       </c>
       <c r="E42" t="s">
-        <v>686</v>
-      </c>
-      <c r="F42" s="34" t="s">
-        <v>687</v>
-      </c>
-      <c r="G42" s="29"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="29"/>
-    </row>
-    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="29">
+        <v>654</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>655</v>
+      </c>
+      <c r="G42" s="30"/>
+      <c r="H42" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="I42" s="30"/>
+    </row>
+    <row r="43" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A43" s="32">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>42</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="C43" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="D43" s="29" t="s">
+      <c r="C43" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="D43" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="E43" s="12" t="s">
-        <v>693</v>
-      </c>
-      <c r="F43" s="29" t="s">
-        <v>702</v>
-      </c>
-      <c r="G43" s="29"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="29"/>
-    </row>
-    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="25">
+      <c r="E43" t="s">
+        <v>636</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="G43" s="30"/>
+      <c r="H43" s="36" t="s">
+        <v>713</v>
+      </c>
+      <c r="I43" s="30"/>
+    </row>
+    <row r="44" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A44" s="26">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>43</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="C44" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="29" t="s">
+      <c r="C44" s="30" t="s">
+        <v>722</v>
+      </c>
+      <c r="D44" s="30" t="s">
         <v>558</v>
       </c>
       <c r="E44" t="s">
-        <v>643</v>
-      </c>
-      <c r="F44" s="29" t="s">
-        <v>644</v>
-      </c>
-      <c r="G44" s="29"/>
-      <c r="H44" s="35" t="s">
-        <v>645</v>
-      </c>
-      <c r="I44" s="29"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="25">
+        <v>723</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="G44" s="30"/>
+      <c r="H44" s="38" t="s">
+        <v>724</v>
+      </c>
+      <c r="I44" s="30"/>
+    </row>
+    <row r="45" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A45" s="30">
         <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
         <v>44</v>
       </c>
-      <c r="B45" s="25" t="s">
-        <v>578</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>578</v>
-      </c>
-      <c r="D45" s="25" t="s">
+      <c r="B45" s="30" t="s">
+        <v>557</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E45" t="s">
+        <v>682</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>683</v>
+      </c>
+      <c r="G45" s="30"/>
+      <c r="H45" s="36" t="s">
+        <v>747</v>
+      </c>
+      <c r="I45" s="30"/>
+    </row>
+    <row r="46" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A46" s="30">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>45</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>557</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>698</v>
+      </c>
+      <c r="G46" s="30"/>
+      <c r="H46" s="38" t="s">
+        <v>725</v>
+      </c>
+      <c r="I46" s="30" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="26">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>46</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>557</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E47" t="s">
+        <v>640</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="G47" s="30"/>
+      <c r="H47" s="36" t="s">
+        <v>642</v>
+      </c>
+      <c r="I47" s="30"/>
+    </row>
+    <row r="48" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+      <c r="A48" s="26">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>47</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>557</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E48" t="s">
+        <v>721</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="G48" s="30"/>
+      <c r="H48" s="38" t="s">
+        <v>726</v>
+      </c>
+      <c r="I48" s="30"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="26">
+        <f>ROW() - ROW(Sala_de_medicacao_e_Internacao!$A$1)</f>
+        <v>48</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>576</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>576</v>
+      </c>
+      <c r="D49" s="26" t="s">
         <v>560</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25" t="s">
-        <v>579</v>
-      </c>
-      <c r="H45" s="31"/>
-      <c r="I45" s="25"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26" t="s">
+        <v>577</v>
+      </c>
+      <c r="H49" s="32"/>
+      <c r="I49" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -10975,7 +11486,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>545</v>
@@ -10999,42 +11510,42 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>